<commit_message>
Sreenivas 10 Oct 2024
</commit_message>
<xml_diff>
--- a/TestResult/BookingOutput.xlsx
+++ b/TestResult/BookingOutput.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3511" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3641" uniqueCount="807">
   <si>
     <t>TestCaseNo</t>
   </si>
@@ -2350,6 +2350,111 @@
   </si>
   <si>
     <t>7bae454d-2839-4d5f-a64d-f8295bd2fcaf</t>
+  </si>
+  <si>
+    <t>ZA12550804</t>
+  </si>
+  <si>
+    <t>911907be-622d-4da4-a681-f717782406d6</t>
+  </si>
+  <si>
+    <t>ZA12550817</t>
+  </si>
+  <si>
+    <t>88d3f0cf-8835-4056-94b7-aab8a8cf9cc6</t>
+  </si>
+  <si>
+    <t>ZA12550830</t>
+  </si>
+  <si>
+    <t>a075fc87-fe78-4109-a502-a8e86c786ada</t>
+  </si>
+  <si>
+    <t>ZA12550838</t>
+  </si>
+  <si>
+    <t>76a37c8c-f4cf-46bf-bb6f-6e6c61789288</t>
+  </si>
+  <si>
+    <t>NG12550844</t>
+  </si>
+  <si>
+    <t>3e3faf3f-595f-4501-ae96-b942f0ecd8d2</t>
+  </si>
+  <si>
+    <t>18:51:38</t>
+  </si>
+  <si>
+    <t>18:51:39</t>
+  </si>
+  <si>
+    <t>18:51:40</t>
+  </si>
+  <si>
+    <t>NG12550889</t>
+  </si>
+  <si>
+    <t>28cc9b50-b41e-427d-9df3-5b3e23008243</t>
+  </si>
+  <si>
+    <t>18:24:49</t>
+  </si>
+  <si>
+    <t>18:24:51</t>
+  </si>
+  <si>
+    <t>18:24:52</t>
+  </si>
+  <si>
+    <t>18:24:53</t>
+  </si>
+  <si>
+    <t>ZA12557861</t>
+  </si>
+  <si>
+    <t>dfe1ff76-27ad-4294-9019-7d191438f33e</t>
+  </si>
+  <si>
+    <t>ZA12557877</t>
+  </si>
+  <si>
+    <t>42d2abb1-ce91-4f1a-86fa-7c348d7b84fa</t>
+  </si>
+  <si>
+    <t>ZA12557885</t>
+  </si>
+  <si>
+    <t>489ccab0-b335-4f94-afe0-40b5dbe81a30</t>
+  </si>
+  <si>
+    <t>NG12557910</t>
+  </si>
+  <si>
+    <t>6c47f2df-1089-43ad-b0eb-c2b27511eb41</t>
+  </si>
+  <si>
+    <t>NG12557916</t>
+  </si>
+  <si>
+    <t>e09b1d56-3307-4bf5-a12e-0973f1a62074</t>
+  </si>
+  <si>
+    <t>NG12557921</t>
+  </si>
+  <si>
+    <t>60193234-c143-4885-a642-ce17af7377a6</t>
+  </si>
+  <si>
+    <t>ZA00182878</t>
+  </si>
+  <si>
+    <t>12db59c9-ef07-4774-adfa-3f59ea47d040</t>
+  </si>
+  <si>
+    <t>ZA00182879</t>
+  </si>
+  <si>
+    <t>54ce1b25-4390-427a-b9c9-354a7cff377e</t>
   </si>
 </sst>
 </file>
@@ -2732,7 +2837,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84E5F12-E39D-4679-9700-19497A69F720}">
-  <dimension ref="A1:G636"/>
+  <dimension ref="A1:G660"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -9406,7 +9511,9 @@
       <c r="E333" t="s" s="0">
         <v>332</v>
       </c>
-      <c r="F333" s="0"/>
+      <c r="F333" t="s" s="0">
+        <v>782</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="s" s="0">
@@ -9424,6 +9531,9 @@
       <c r="E334" t="s" s="0">
         <v>334</v>
       </c>
+      <c r="F334" t="s" s="0">
+        <v>783</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="s" s="0">
@@ -9441,6 +9551,9 @@
       <c r="E335" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="F335" t="s" s="0">
+        <v>783</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="s" s="0">
@@ -9458,6 +9571,9 @@
       <c r="E336" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="F336" t="s" s="0">
+        <v>784</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="s" s="0">
@@ -9475,6 +9591,9 @@
       <c r="E337" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="F337" t="s" s="0">
+        <v>784</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="s" s="0">
@@ -9492,6 +9611,9 @@
       <c r="E338" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="F338" t="s" s="0">
+        <v>787</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="s" s="0">
@@ -9509,6 +9631,9 @@
       <c r="E339" t="s" s="0">
         <v>340</v>
       </c>
+      <c r="F339" t="s" s="0">
+        <v>788</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="s" s="0">
@@ -9526,6 +9651,9 @@
       <c r="E340" t="s" s="0">
         <v>342</v>
       </c>
+      <c r="F340" t="s" s="0">
+        <v>789</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="s" s="0">
@@ -9543,6 +9671,9 @@
       <c r="E341" t="s" s="0">
         <v>344</v>
       </c>
+      <c r="F341" t="s" s="0">
+        <v>789</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="s" s="0">
@@ -9560,6 +9691,9 @@
       <c r="E342" t="s" s="0">
         <v>346</v>
       </c>
+      <c r="F342" t="s" s="0">
+        <v>790</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="s" s="0">
@@ -9577,6 +9711,7 @@
       <c r="E343" t="s" s="0">
         <v>348</v>
       </c>
+      <c r="F343" s="0"/>
     </row>
     <row r="344">
       <c r="A344" t="s" s="0">
@@ -14535,6 +14670,9 @@
       <c r="C635" t="s" s="0">
         <v>17</v>
       </c>
+      <c r="D635" t="s" s="0">
+        <v>18</v>
+      </c>
       <c r="E635" t="s" s="0">
         <v>769</v>
       </c>
@@ -14549,8 +14687,413 @@
       <c r="C636" t="s" s="0">
         <v>17</v>
       </c>
+      <c r="D636" t="s" s="0">
+        <v>18</v>
+      </c>
       <c r="E636" t="s" s="0">
         <v>771</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B637" t="s" s="0">
+        <v>772</v>
+      </c>
+      <c r="C637" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D637" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E637" t="s" s="0">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B638" t="s" s="0">
+        <v>774</v>
+      </c>
+      <c r="C638" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D638" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E638" t="s" s="0">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B639" t="s" s="0">
+        <v>776</v>
+      </c>
+      <c r="C639" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D639" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E639" t="s" s="0">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B640" t="s" s="0">
+        <v>778</v>
+      </c>
+      <c r="C640" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D640" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E640" t="s" s="0">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B641" t="s" s="0">
+        <v>780</v>
+      </c>
+      <c r="C641" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D641" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E641" t="s" s="0">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B642" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C642" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D642" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E642" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B643" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C643" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D643" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E643" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B644" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C644" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D644" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E644" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B645" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C645" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D645" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E645" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B646" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C646" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D646" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E646" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B647" t="s" s="0">
+        <v>785</v>
+      </c>
+      <c r="C647" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D647" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E647" t="s" s="0">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B648" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C648" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D648" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E648" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B649" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C649" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D649" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E649" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B650" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C650" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D650" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E650" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B651" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C651" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D651" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E651" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B652" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C652" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D652" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E652" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B653" t="s" s="0">
+        <v>791</v>
+      </c>
+      <c r="C653" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D653" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E653" t="s" s="0">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B654" t="s" s="0">
+        <v>793</v>
+      </c>
+      <c r="C654" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D654" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E654" t="s" s="0">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B655" t="s" s="0">
+        <v>795</v>
+      </c>
+      <c r="C655" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D655" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E655" t="s" s="0">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B656" t="s" s="0">
+        <v>797</v>
+      </c>
+      <c r="C656" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D656" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E656" t="s" s="0">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B657" t="s" s="0">
+        <v>799</v>
+      </c>
+      <c r="C657" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D657" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E657" t="s" s="0">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B658" t="s" s="0">
+        <v>801</v>
+      </c>
+      <c r="C658" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D658" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E658" t="s" s="0">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B659" t="s" s="0">
+        <v>803</v>
+      </c>
+      <c r="C659" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E659" t="s" s="0">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B660" t="s" s="0">
+        <v>805</v>
+      </c>
+      <c r="C660" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E660" t="s" s="0">
+        <v>806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>